<commit_message>
tien commit sua thong bao
</commit_message>
<xml_diff>
--- a/file/datachuyennganh.xlsx
+++ b/file/datachuyennganh.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\data_baitaplon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPTOP\Desktop\HK1-Nam4\Cong nghe moi\Do an\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51682895-A3CD-4783-BDAF-0B9EDA95F69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEC1186-4DED-4B8A-B32E-CB73724B6342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,10 +48,10 @@
     <t>Mã khoa</t>
   </si>
   <si>
+    <t>Hha</t>
+  </si>
+  <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>KTKT</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,10 +414,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
@@ -428,10 +428,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1"/>
@@ -442,10 +442,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
@@ -456,10 +456,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="1"/>

</xml_diff>